<commit_message>
updated mapping-file-set/system-of-record-mapping-no-grid.xlsx.  will update more tonight
</commit_message>
<xml_diff>
--- a/source-code/scratch/owin/mmrds-importer/mapping-file-set/system-of-record-mapping-no-grid.xlsx
+++ b/source-code/scratch/owin/mmrds-importer/mapping-file-set/system-of-record-mapping-no-grid.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8352"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20160" windowHeight="7992"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet5" sheetId="5" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6080" uniqueCount="2495">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6081" uniqueCount="2496">
   <si>
     <t>Path</t>
   </si>
@@ -6631,9 +6631,6 @@
     <t>birth_fetal_death_certificate_parent/cigarette_smoking/none_or_not_specified</t>
   </si>
   <si>
-    <t>Need to add field for not specified- none and not specified are not the same</t>
-  </si>
-  <si>
     <t>birth_fetal_death_certificate_parent/reviewer_note</t>
   </si>
   <si>
@@ -7529,6 +7526,12 @@
   </si>
   <si>
     <t>death_certificate/address_of_death/county</t>
+  </si>
+  <si>
+    <t>birth_fetal_death_certificate_parent/risk_factors/number_of_c_sections</t>
+  </si>
+  <si>
+    <t>birth_fetal_death_certificate_parent/location_of_residence/estimated_distance_from_residence</t>
   </si>
 </sst>
 </file>
@@ -8079,8 +8082,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K776"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B199" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="B525" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="H526" sqref="H526"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10370,7 +10373,7 @@
         <v>7</v>
       </c>
       <c r="H88" s="6" t="s">
-        <v>2417</v>
+        <v>2416</v>
       </c>
     </row>
     <row r="89" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
@@ -10442,7 +10445,7 @@
         <v>28</v>
       </c>
       <c r="H91" s="6" t="s">
-        <v>2418</v>
+        <v>2417</v>
       </c>
     </row>
     <row r="92" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -10468,7 +10471,7 @@
         <v>28</v>
       </c>
       <c r="H92" s="6" t="s">
-        <v>2418</v>
+        <v>2417</v>
       </c>
     </row>
     <row r="93" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -10517,7 +10520,7 @@
         <v>56</v>
       </c>
       <c r="H94" s="6" t="s">
-        <v>2419</v>
+        <v>2418</v>
       </c>
     </row>
     <row r="95" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -10543,7 +10546,7 @@
         <v>11</v>
       </c>
       <c r="J95" s="14" t="s">
-        <v>2420</v>
+        <v>2419</v>
       </c>
     </row>
     <row r="96" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -10569,7 +10572,7 @@
         <v>7</v>
       </c>
       <c r="H96" s="6" t="s">
-        <v>2421</v>
+        <v>2420</v>
       </c>
     </row>
     <row r="97" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -10595,7 +10598,7 @@
         <v>56</v>
       </c>
       <c r="J97" s="14" t="s">
-        <v>2266</v>
+        <v>2265</v>
       </c>
     </row>
     <row r="98" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -10621,7 +10624,7 @@
         <v>28</v>
       </c>
       <c r="H98" s="6" t="s">
-        <v>2422</v>
+        <v>2421</v>
       </c>
     </row>
     <row r="99" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -10648,7 +10651,7 @@
       </c>
       <c r="H99" s="17"/>
       <c r="J99" s="14" t="s">
-        <v>2423</v>
+        <v>2422</v>
       </c>
     </row>
     <row r="100" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -10674,7 +10677,7 @@
         <v>28</v>
       </c>
       <c r="H100" s="6" t="s">
-        <v>2422</v>
+        <v>2421</v>
       </c>
     </row>
     <row r="101" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -10700,7 +10703,7 @@
         <v>28</v>
       </c>
       <c r="H101" s="6" t="s">
-        <v>2422</v>
+        <v>2421</v>
       </c>
     </row>
     <row r="102" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
@@ -10726,7 +10729,7 @@
         <v>28</v>
       </c>
       <c r="H102" s="6" t="s">
-        <v>2422</v>
+        <v>2421</v>
       </c>
     </row>
     <row r="103" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -10752,7 +10755,7 @@
         <v>56</v>
       </c>
       <c r="J103" s="14" t="s">
-        <v>2266</v>
+        <v>2265</v>
       </c>
     </row>
     <row r="104" spans="1:10" ht="72" x14ac:dyDescent="0.3">
@@ -10778,7 +10781,7 @@
         <v>56</v>
       </c>
       <c r="H104" s="6" t="s">
-        <v>2424</v>
+        <v>2423</v>
       </c>
     </row>
     <row r="105" spans="1:10" x14ac:dyDescent="0.3">
@@ -11116,7 +11119,7 @@
         <v>11</v>
       </c>
       <c r="H117" s="22" t="s">
-        <v>2489</v>
+        <v>2488</v>
       </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.3">
@@ -11492,7 +11495,7 @@
         <v>56</v>
       </c>
       <c r="H132" s="22" t="s">
-        <v>2491</v>
+        <v>2490</v>
       </c>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.3">
@@ -11700,7 +11703,7 @@
         <v>56</v>
       </c>
       <c r="H140" s="22" t="s">
-        <v>2486</v>
+        <v>2485</v>
       </c>
     </row>
     <row r="141" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -11752,7 +11755,7 @@
         <v>56</v>
       </c>
       <c r="H142" s="22" t="s">
-        <v>2494</v>
+        <v>2493</v>
       </c>
     </row>
     <row r="143" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -11960,7 +11963,7 @@
         <v>11</v>
       </c>
       <c r="H150" s="22" t="s">
-        <v>2488</v>
+        <v>2487</v>
       </c>
       <c r="J150" s="6"/>
     </row>
@@ -12192,7 +12195,7 @@
         <v>56</v>
       </c>
       <c r="H159" s="22" t="s">
-        <v>2492</v>
+        <v>2491</v>
       </c>
     </row>
     <row r="160" spans="1:10" x14ac:dyDescent="0.3">
@@ -12351,7 +12354,7 @@
         <v>56</v>
       </c>
       <c r="H165" s="22" t="s">
-        <v>2493</v>
+        <v>2492</v>
       </c>
     </row>
     <row r="166" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -12579,7 +12582,7 @@
         <v>56</v>
       </c>
       <c r="H174" s="22" t="s">
-        <v>2485</v>
+        <v>2484</v>
       </c>
     </row>
     <row r="175" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -12787,7 +12790,7 @@
         <v>56</v>
       </c>
       <c r="H182" s="22" t="s">
-        <v>2487</v>
+        <v>2486</v>
       </c>
     </row>
     <row r="183" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -13019,7 +13022,7 @@
         <v>11</v>
       </c>
       <c r="H191" s="22" t="s">
-        <v>2490</v>
+        <v>2489</v>
       </c>
       <c r="J191" s="6"/>
     </row>
@@ -13046,7 +13049,7 @@
         <v>7</v>
       </c>
       <c r="H192" s="6" t="s">
-        <v>2468</v>
+        <v>2467</v>
       </c>
     </row>
     <row r="193" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -13072,7 +13075,7 @@
         <v>7</v>
       </c>
       <c r="H193" s="6" t="s">
-        <v>2469</v>
+        <v>2468</v>
       </c>
     </row>
     <row r="194" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -13098,7 +13101,7 @@
         <v>7</v>
       </c>
       <c r="H194" s="6" t="s">
-        <v>2470</v>
+        <v>2469</v>
       </c>
     </row>
     <row r="195" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -13124,7 +13127,7 @@
         <v>328</v>
       </c>
       <c r="H195" s="6" t="s">
-        <v>2471</v>
+        <v>2470</v>
       </c>
     </row>
     <row r="196" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -13244,7 +13247,7 @@
         <v>328</v>
       </c>
       <c r="H200" s="6" t="s">
-        <v>2472</v>
+        <v>2471</v>
       </c>
     </row>
     <row r="201" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -13270,7 +13273,7 @@
         <v>56</v>
       </c>
       <c r="H201" s="6" t="s">
-        <v>2425</v>
+        <v>2424</v>
       </c>
     </row>
     <row r="202" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -13296,7 +13299,7 @@
         <v>11</v>
       </c>
       <c r="H202" s="6" t="s">
-        <v>2426</v>
+        <v>2425</v>
       </c>
     </row>
     <row r="203" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -13322,7 +13325,7 @@
         <v>11</v>
       </c>
       <c r="H203" s="6" t="s">
-        <v>2429</v>
+        <v>2428</v>
       </c>
     </row>
     <row r="204" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -13394,7 +13397,7 @@
         <v>11</v>
       </c>
       <c r="H206" s="6" t="s">
-        <v>2432</v>
+        <v>2431</v>
       </c>
     </row>
     <row r="207" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -13420,7 +13423,7 @@
         <v>11</v>
       </c>
       <c r="H207" s="6" t="s">
-        <v>2437</v>
+        <v>2436</v>
       </c>
     </row>
     <row r="208" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -13446,7 +13449,7 @@
         <v>28</v>
       </c>
       <c r="H208" s="6" t="s">
-        <v>2438</v>
+        <v>2437</v>
       </c>
     </row>
     <row r="209" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -13472,7 +13475,7 @@
         <v>7</v>
       </c>
       <c r="H209" s="6" t="s">
-        <v>2439</v>
+        <v>2438</v>
       </c>
     </row>
     <row r="210" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -13498,7 +13501,7 @@
         <v>11</v>
       </c>
       <c r="H210" s="6" t="s">
-        <v>2440</v>
+        <v>2439</v>
       </c>
     </row>
     <row r="211" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -13524,7 +13527,7 @@
         <v>11</v>
       </c>
       <c r="H211" s="6" t="s">
-        <v>2441</v>
+        <v>2440</v>
       </c>
     </row>
     <row r="212" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -13688,7 +13691,7 @@
         <v>11</v>
       </c>
       <c r="H218" s="6" t="s">
-        <v>2444</v>
+        <v>2443</v>
       </c>
     </row>
     <row r="219" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -13783,7 +13786,7 @@
         <v>56</v>
       </c>
       <c r="H222" s="6" t="s">
-        <v>2446</v>
+        <v>2445</v>
       </c>
     </row>
     <row r="223" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -13809,7 +13812,7 @@
         <v>56</v>
       </c>
       <c r="H223" s="6" t="s">
-        <v>2445</v>
+        <v>2444</v>
       </c>
     </row>
     <row r="224" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -13835,7 +13838,7 @@
         <v>56</v>
       </c>
       <c r="H224" s="6" t="s">
-        <v>2447</v>
+        <v>2446</v>
       </c>
     </row>
     <row r="225" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -13861,7 +13864,7 @@
         <v>11</v>
       </c>
       <c r="H225" s="6" t="s">
-        <v>2448</v>
+        <v>2447</v>
       </c>
     </row>
     <row r="226" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -13887,7 +13890,7 @@
         <v>11</v>
       </c>
       <c r="H226" s="6" t="s">
-        <v>2449</v>
+        <v>2448</v>
       </c>
     </row>
     <row r="227" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -13913,7 +13916,7 @@
         <v>11</v>
       </c>
       <c r="H227" s="8" t="s">
-        <v>2230</v>
+        <v>2229</v>
       </c>
     </row>
     <row r="228" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -13939,7 +13942,7 @@
         <v>11</v>
       </c>
       <c r="H228" s="8" t="s">
-        <v>2231</v>
+        <v>2230</v>
       </c>
     </row>
     <row r="229" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -14011,7 +14014,7 @@
         <v>56</v>
       </c>
       <c r="H231" s="8" t="s">
-        <v>2450</v>
+        <v>2449</v>
       </c>
     </row>
     <row r="232" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -14037,7 +14040,7 @@
         <v>11</v>
       </c>
       <c r="H232" s="6" t="s">
-        <v>2427</v>
+        <v>2426</v>
       </c>
     </row>
     <row r="233" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -14063,7 +14066,7 @@
         <v>11</v>
       </c>
       <c r="H233" s="6" t="s">
-        <v>2430</v>
+        <v>2429</v>
       </c>
     </row>
     <row r="234" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -14089,7 +14092,7 @@
         <v>11</v>
       </c>
       <c r="H234" s="6" t="s">
-        <v>2433</v>
+        <v>2432</v>
       </c>
     </row>
     <row r="235" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -14115,7 +14118,7 @@
         <v>11</v>
       </c>
       <c r="H235" s="6" t="s">
-        <v>2436</v>
+        <v>2435</v>
       </c>
     </row>
     <row r="236" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -14164,7 +14167,7 @@
         <v>11</v>
       </c>
       <c r="H237" s="6" t="s">
-        <v>2442</v>
+        <v>2441</v>
       </c>
     </row>
     <row r="238" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -14213,7 +14216,7 @@
         <v>56</v>
       </c>
       <c r="H239" s="8" t="s">
-        <v>2451</v>
+        <v>2450</v>
       </c>
     </row>
     <row r="240" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -14239,7 +14242,7 @@
         <v>56</v>
       </c>
       <c r="H240" s="8" t="s">
-        <v>2452</v>
+        <v>2451</v>
       </c>
     </row>
     <row r="241" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -14265,7 +14268,7 @@
         <v>56</v>
       </c>
       <c r="H241" s="8" t="s">
-        <v>2453</v>
+        <v>2452</v>
       </c>
     </row>
     <row r="242" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
@@ -14291,7 +14294,7 @@
         <v>7</v>
       </c>
       <c r="H242" s="9" t="s">
-        <v>2454</v>
+        <v>2453</v>
       </c>
     </row>
     <row r="243" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -14343,7 +14346,7 @@
         <v>7</v>
       </c>
       <c r="H244" s="6" t="s">
-        <v>2473</v>
+        <v>2472</v>
       </c>
     </row>
     <row r="245" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -14369,7 +14372,7 @@
         <v>7</v>
       </c>
       <c r="H245" s="6" t="s">
-        <v>2474</v>
+        <v>2473</v>
       </c>
     </row>
     <row r="246" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -14395,7 +14398,7 @@
         <v>56</v>
       </c>
       <c r="J246" s="14" t="s">
-        <v>2266</v>
+        <v>2265</v>
       </c>
     </row>
     <row r="247" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
@@ -14421,7 +14424,7 @@
         <v>56</v>
       </c>
       <c r="H247" s="8" t="s">
-        <v>2455</v>
+        <v>2454</v>
       </c>
     </row>
     <row r="248" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -14447,7 +14450,7 @@
         <v>7</v>
       </c>
       <c r="H248" s="6" t="s">
-        <v>2456</v>
+        <v>2455</v>
       </c>
     </row>
     <row r="249" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -14615,7 +14618,7 @@
         <v>7</v>
       </c>
       <c r="H255" s="6" t="s">
-        <v>2457</v>
+        <v>2456</v>
       </c>
     </row>
     <row r="256" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
@@ -14641,7 +14644,7 @@
         <v>7</v>
       </c>
       <c r="H256" s="6" t="s">
-        <v>2475</v>
+        <v>2474</v>
       </c>
     </row>
     <row r="257" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -14667,7 +14670,7 @@
         <v>56</v>
       </c>
       <c r="H257" s="8" t="s">
-        <v>2458</v>
+        <v>2457</v>
       </c>
     </row>
     <row r="258" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -14693,7 +14696,7 @@
         <v>56</v>
       </c>
       <c r="H258" s="8" t="s">
-        <v>2459</v>
+        <v>2458</v>
       </c>
     </row>
     <row r="259" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -14719,7 +14722,7 @@
         <v>11</v>
       </c>
       <c r="H259" s="8" t="s">
-        <v>2460</v>
+        <v>2459</v>
       </c>
     </row>
     <row r="260" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -14745,7 +14748,7 @@
         <v>11</v>
       </c>
       <c r="H260" s="8" t="s">
-        <v>2461</v>
+        <v>2460</v>
       </c>
     </row>
     <row r="261" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -14771,7 +14774,7 @@
         <v>7</v>
       </c>
       <c r="H261" s="9" t="s">
-        <v>2476</v>
+        <v>2475</v>
       </c>
     </row>
     <row r="262" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -14797,7 +14800,7 @@
         <v>56</v>
       </c>
       <c r="H262" s="8" t="s">
-        <v>2462</v>
+        <v>2461</v>
       </c>
     </row>
     <row r="263" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -14823,7 +14826,7 @@
         <v>56</v>
       </c>
       <c r="H263" s="8" t="s">
-        <v>2463</v>
+        <v>2462</v>
       </c>
     </row>
     <row r="264" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -14849,7 +14852,7 @@
         <v>56</v>
       </c>
       <c r="J264" s="14" t="s">
-        <v>2266</v>
+        <v>2265</v>
       </c>
     </row>
     <row r="265" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -14898,7 +14901,7 @@
         <v>28</v>
       </c>
       <c r="H266" s="6" t="s">
-        <v>2464</v>
+        <v>2463</v>
       </c>
     </row>
     <row r="267" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -14924,7 +14927,7 @@
         <v>28</v>
       </c>
       <c r="H267" s="6" t="s">
-        <v>2465</v>
+        <v>2464</v>
       </c>
     </row>
     <row r="268" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -14973,7 +14976,7 @@
         <v>328</v>
       </c>
       <c r="H269" s="6" t="s">
-        <v>2477</v>
+        <v>2476</v>
       </c>
     </row>
     <row r="270" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
@@ -14999,7 +15002,7 @@
         <v>263</v>
       </c>
       <c r="H270" s="6" t="s">
-        <v>2478</v>
+        <v>2477</v>
       </c>
     </row>
     <row r="271" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
@@ -15025,7 +15028,7 @@
         <v>263</v>
       </c>
       <c r="H271" s="6" t="s">
-        <v>2479</v>
+        <v>2478</v>
       </c>
     </row>
     <row r="272" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -15074,7 +15077,7 @@
         <v>263</v>
       </c>
       <c r="H273" s="6" t="s">
-        <v>2480</v>
+        <v>2479</v>
       </c>
     </row>
     <row r="274" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -15100,7 +15103,7 @@
         <v>56</v>
       </c>
       <c r="H274" s="6" t="s">
-        <v>2466</v>
+        <v>2465</v>
       </c>
     </row>
     <row r="275" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
@@ -15126,7 +15129,7 @@
         <v>7</v>
       </c>
       <c r="H275" s="6" t="s">
-        <v>2481</v>
+        <v>2480</v>
       </c>
     </row>
     <row r="276" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -15152,7 +15155,7 @@
         <v>7</v>
       </c>
       <c r="H276" s="6" t="s">
-        <v>2482</v>
+        <v>2481</v>
       </c>
     </row>
     <row r="277" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
@@ -15178,7 +15181,7 @@
         <v>11</v>
       </c>
       <c r="H277" s="6" t="s">
-        <v>2484</v>
+        <v>2483</v>
       </c>
     </row>
     <row r="278" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -15204,7 +15207,7 @@
         <v>7</v>
       </c>
       <c r="H278" s="6" t="s">
-        <v>2483</v>
+        <v>2482</v>
       </c>
     </row>
     <row r="279" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -15230,7 +15233,7 @@
         <v>263</v>
       </c>
       <c r="H279" s="8" t="s">
-        <v>2480</v>
+        <v>2479</v>
       </c>
     </row>
     <row r="280" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -15256,7 +15259,7 @@
         <v>7</v>
       </c>
       <c r="H280" s="6" t="s">
-        <v>2467</v>
+        <v>2466</v>
       </c>
     </row>
     <row r="281" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -15305,7 +15308,7 @@
         <v>11</v>
       </c>
       <c r="H282" s="6" t="s">
-        <v>2428</v>
+        <v>2427</v>
       </c>
     </row>
     <row r="283" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
@@ -15331,7 +15334,7 @@
         <v>11</v>
       </c>
       <c r="H283" s="6" t="s">
-        <v>2431</v>
+        <v>2430</v>
       </c>
     </row>
     <row r="284" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -15357,7 +15360,7 @@
         <v>11</v>
       </c>
       <c r="H284" s="6" t="s">
-        <v>2434</v>
+        <v>2433</v>
       </c>
     </row>
     <row r="285" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -15383,7 +15386,7 @@
         <v>11</v>
       </c>
       <c r="H285" s="6" t="s">
-        <v>2435</v>
+        <v>2434</v>
       </c>
     </row>
     <row r="286" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
@@ -15409,7 +15412,7 @@
         <v>11</v>
       </c>
       <c r="H286" s="6" t="s">
-        <v>2443</v>
+        <v>2442</v>
       </c>
     </row>
     <row r="287" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -15435,7 +15438,7 @@
         <v>7</v>
       </c>
       <c r="H287" s="6" t="s">
-        <v>2287</v>
+        <v>2286</v>
       </c>
     </row>
     <row r="288" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -15462,10 +15465,10 @@
       </c>
       <c r="H288" s="17"/>
       <c r="I288" s="6" t="s">
+        <v>2287</v>
+      </c>
+      <c r="J288" s="14" t="s">
         <v>2288</v>
-      </c>
-      <c r="J288" s="14" t="s">
-        <v>2289</v>
       </c>
     </row>
     <row r="289" spans="1:10" x14ac:dyDescent="0.3">
@@ -15537,7 +15540,7 @@
         <v>7</v>
       </c>
       <c r="H291" s="6" t="s">
-        <v>2290</v>
+        <v>2289</v>
       </c>
     </row>
     <row r="292" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -15563,7 +15566,7 @@
         <v>28</v>
       </c>
       <c r="H292" s="6" t="s">
-        <v>2291</v>
+        <v>2290</v>
       </c>
     </row>
     <row r="293" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -15589,7 +15592,7 @@
         <v>28</v>
       </c>
       <c r="H293" s="6" t="s">
-        <v>2291</v>
+        <v>2290</v>
       </c>
     </row>
     <row r="294" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -15615,7 +15618,7 @@
         <v>28</v>
       </c>
       <c r="H294" s="6" t="s">
-        <v>2291</v>
+        <v>2290</v>
       </c>
     </row>
     <row r="295" spans="1:10" x14ac:dyDescent="0.3">
@@ -15641,7 +15644,7 @@
         <v>56</v>
       </c>
       <c r="H295" s="6" t="s">
-        <v>2293</v>
+        <v>2292</v>
       </c>
     </row>
     <row r="296" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -15667,7 +15670,7 @@
         <v>7</v>
       </c>
       <c r="H296" s="6" t="s">
-        <v>2296</v>
+        <v>2295</v>
       </c>
     </row>
     <row r="297" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -15694,10 +15697,10 @@
       </c>
       <c r="H297" s="17"/>
       <c r="I297" s="6" t="s">
+        <v>2287</v>
+      </c>
+      <c r="J297" s="14" t="s">
         <v>2288</v>
-      </c>
-      <c r="J297" s="14" t="s">
-        <v>2289</v>
       </c>
     </row>
     <row r="298" spans="1:10" x14ac:dyDescent="0.3">
@@ -15723,7 +15726,7 @@
         <v>56</v>
       </c>
       <c r="H298" s="6" t="s">
-        <v>2293</v>
+        <v>2292</v>
       </c>
     </row>
     <row r="299" spans="1:10" x14ac:dyDescent="0.3">
@@ -15749,7 +15752,7 @@
         <v>56</v>
       </c>
       <c r="H299" s="6" t="s">
-        <v>2292</v>
+        <v>2291</v>
       </c>
     </row>
     <row r="300" spans="1:10" x14ac:dyDescent="0.3">
@@ -15775,7 +15778,7 @@
         <v>56</v>
       </c>
       <c r="H300" s="6" t="s">
-        <v>2294</v>
+        <v>2293</v>
       </c>
     </row>
     <row r="301" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -15801,7 +15804,7 @@
         <v>7</v>
       </c>
       <c r="H301" s="6" t="s">
-        <v>2295</v>
+        <v>2294</v>
       </c>
     </row>
     <row r="302" spans="1:10" x14ac:dyDescent="0.3">
@@ -15827,7 +15830,7 @@
         <v>56</v>
       </c>
       <c r="J302" s="14" t="s">
-        <v>2266</v>
+        <v>2265</v>
       </c>
     </row>
     <row r="303" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -15853,7 +15856,7 @@
         <v>7</v>
       </c>
       <c r="H303" s="6" t="s">
-        <v>2291</v>
+        <v>2290</v>
       </c>
     </row>
     <row r="304" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -15880,10 +15883,10 @@
       </c>
       <c r="H304" s="17"/>
       <c r="I304" s="6" t="s">
+        <v>2287</v>
+      </c>
+      <c r="J304" s="14" t="s">
         <v>2288</v>
-      </c>
-      <c r="J304" s="14" t="s">
-        <v>2289</v>
       </c>
     </row>
     <row r="305" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -16340,7 +16343,7 @@
         <v>11</v>
       </c>
       <c r="H322" s="8" t="s">
-        <v>2245</v>
+        <v>2244</v>
       </c>
     </row>
     <row r="323" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -16366,7 +16369,7 @@
         <v>11</v>
       </c>
       <c r="H323" s="6" t="s">
-        <v>2247</v>
+        <v>2246</v>
       </c>
     </row>
     <row r="324" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
@@ -16393,7 +16396,7 @@
       </c>
       <c r="H324" s="17"/>
       <c r="J324" s="21" t="s">
-        <v>2257</v>
+        <v>2256</v>
       </c>
     </row>
     <row r="325" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -16420,7 +16423,7 @@
       </c>
       <c r="H325" s="17"/>
       <c r="I325" s="6" t="s">
-        <v>2246</v>
+        <v>2245</v>
       </c>
     </row>
     <row r="326" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -16447,7 +16450,7 @@
       </c>
       <c r="H326" s="17"/>
       <c r="I326" s="6" t="s">
-        <v>2249</v>
+        <v>2248</v>
       </c>
     </row>
     <row r="327" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -16474,7 +16477,7 @@
       </c>
       <c r="H327" s="17"/>
       <c r="I327" s="6" t="s">
-        <v>2248</v>
+        <v>2247</v>
       </c>
     </row>
     <row r="328" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -16500,7 +16503,7 @@
         <v>11</v>
       </c>
       <c r="H328" s="6" t="s">
-        <v>2284</v>
+        <v>2283</v>
       </c>
     </row>
     <row r="329" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -16526,7 +16529,7 @@
         <v>11</v>
       </c>
       <c r="H329" s="6" t="s">
-        <v>2285</v>
+        <v>2284</v>
       </c>
     </row>
     <row r="330" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -16786,7 +16789,7 @@
         <v>56</v>
       </c>
       <c r="H340" s="8" t="s">
-        <v>2216</v>
+        <v>2215</v>
       </c>
     </row>
     <row r="341" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -16812,7 +16815,7 @@
         <v>56</v>
       </c>
       <c r="H341" s="8" t="s">
-        <v>2217</v>
+        <v>2216</v>
       </c>
     </row>
     <row r="342" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -16838,7 +16841,7 @@
         <v>11</v>
       </c>
       <c r="H342" s="6" t="s">
-        <v>2218</v>
+        <v>2217</v>
       </c>
     </row>
     <row r="343" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -16942,7 +16945,7 @@
         <v>56</v>
       </c>
       <c r="H346" s="6" t="s">
-        <v>2219</v>
+        <v>2218</v>
       </c>
     </row>
     <row r="347" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -16968,7 +16971,7 @@
         <v>7</v>
       </c>
       <c r="H347" s="6" t="s">
-        <v>2220</v>
+        <v>2219</v>
       </c>
     </row>
     <row r="348" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -16994,7 +16997,7 @@
         <v>7</v>
       </c>
       <c r="H348" s="6" t="s">
-        <v>2221</v>
+        <v>2220</v>
       </c>
     </row>
     <row r="349" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -17092,7 +17095,7 @@
         <v>7</v>
       </c>
       <c r="H352" s="6" t="s">
-        <v>2222</v>
+        <v>2221</v>
       </c>
     </row>
     <row r="353" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
@@ -17170,7 +17173,7 @@
         <v>56</v>
       </c>
       <c r="H355" s="6" t="s">
-        <v>2223</v>
+        <v>2222</v>
       </c>
     </row>
     <row r="356" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -17222,7 +17225,7 @@
         <v>7</v>
       </c>
       <c r="H357" s="6" t="s">
-        <v>2224</v>
+        <v>2223</v>
       </c>
     </row>
     <row r="358" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -17300,7 +17303,7 @@
         <v>56</v>
       </c>
       <c r="H360" s="6" t="s">
-        <v>2225</v>
+        <v>2224</v>
       </c>
     </row>
     <row r="361" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -17326,7 +17329,7 @@
         <v>56</v>
       </c>
       <c r="H361" s="6" t="s">
-        <v>2226</v>
+        <v>2225</v>
       </c>
     </row>
     <row r="362" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -17378,7 +17381,7 @@
         <v>56</v>
       </c>
       <c r="H363" s="6" t="s">
-        <v>2227</v>
+        <v>2226</v>
       </c>
     </row>
     <row r="364" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -17609,7 +17612,7 @@
         <v>56</v>
       </c>
       <c r="H372" s="6" t="s">
-        <v>2228</v>
+        <v>2227</v>
       </c>
     </row>
     <row r="373" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -17895,7 +17898,7 @@
         <v>7</v>
       </c>
       <c r="H383" s="6" t="s">
-        <v>2229</v>
+        <v>2228</v>
       </c>
     </row>
     <row r="384" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -17921,7 +17924,7 @@
         <v>11</v>
       </c>
       <c r="H384" s="6" t="s">
-        <v>2230</v>
+        <v>2229</v>
       </c>
     </row>
     <row r="385" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -17947,7 +17950,7 @@
         <v>11</v>
       </c>
       <c r="H385" s="6" t="s">
-        <v>2231</v>
+        <v>2230</v>
       </c>
     </row>
     <row r="386" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -18127,7 +18130,7 @@
         <v>11</v>
       </c>
       <c r="H392" s="6" t="s">
-        <v>2239</v>
+        <v>2238</v>
       </c>
     </row>
     <row r="393" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -18153,7 +18156,7 @@
         <v>11</v>
       </c>
       <c r="H393" s="6" t="s">
-        <v>2240</v>
+        <v>2239</v>
       </c>
     </row>
     <row r="394" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -18179,7 +18182,7 @@
         <v>11</v>
       </c>
       <c r="H394" s="6" t="s">
-        <v>2241</v>
+        <v>2240</v>
       </c>
     </row>
     <row r="395" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -18309,7 +18312,7 @@
         <v>11</v>
       </c>
       <c r="H399" s="8" t="s">
-        <v>2242</v>
+        <v>2241</v>
       </c>
     </row>
     <row r="400" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -18463,7 +18466,7 @@
         <v>11</v>
       </c>
       <c r="H405" s="6" t="s">
-        <v>2244</v>
+        <v>2243</v>
       </c>
     </row>
     <row r="406" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -18541,7 +18544,7 @@
         <v>56</v>
       </c>
       <c r="H408" s="8" t="s">
-        <v>2243</v>
+        <v>2242</v>
       </c>
     </row>
     <row r="409" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -18594,10 +18597,10 @@
       </c>
       <c r="H410" s="7"/>
       <c r="I410" s="6" t="s">
-        <v>2247</v>
+        <v>2246</v>
       </c>
       <c r="J410" s="14" t="s">
-        <v>2259</v>
+        <v>2258</v>
       </c>
     </row>
     <row r="411" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
@@ -18624,7 +18627,7 @@
       </c>
       <c r="H411" s="17"/>
       <c r="J411" s="21" t="s">
-        <v>2257</v>
+        <v>2256</v>
       </c>
     </row>
     <row r="412" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -18651,10 +18654,10 @@
       </c>
       <c r="H412" s="17"/>
       <c r="I412" s="6" t="s">
-        <v>2246</v>
+        <v>2245</v>
       </c>
       <c r="J412" s="14" t="s">
-        <v>2260</v>
+        <v>2259</v>
       </c>
     </row>
     <row r="413" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -18680,7 +18683,7 @@
         <v>11</v>
       </c>
       <c r="H413" s="6" t="s">
-        <v>2283</v>
+        <v>2282</v>
       </c>
       <c r="I413" s="6"/>
     </row>
@@ -18707,13 +18710,13 @@
         <v>11</v>
       </c>
       <c r="H414" s="6" t="s">
-        <v>2282</v>
+        <v>2281</v>
       </c>
       <c r="I414" s="6" t="s">
-        <v>2248</v>
+        <v>2247</v>
       </c>
       <c r="J414" s="14" t="s">
-        <v>2261</v>
+        <v>2260</v>
       </c>
     </row>
     <row r="415" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -18811,7 +18814,7 @@
         <v>7</v>
       </c>
       <c r="H418" s="6" t="s">
-        <v>2262</v>
+        <v>2261</v>
       </c>
     </row>
     <row r="419" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -18837,7 +18840,7 @@
         <v>7</v>
       </c>
       <c r="H419" s="6" t="s">
-        <v>2263</v>
+        <v>2262</v>
       </c>
     </row>
     <row r="420" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -18864,10 +18867,10 @@
       </c>
       <c r="H420" s="17"/>
       <c r="I420" s="6" t="s">
+        <v>2263</v>
+      </c>
+      <c r="J420" s="14" t="s">
         <v>2264</v>
-      </c>
-      <c r="J420" s="14" t="s">
-        <v>2265</v>
       </c>
     </row>
     <row r="421" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -18969,7 +18972,7 @@
         <v>7</v>
       </c>
       <c r="H424" s="6" t="s">
-        <v>2267</v>
+        <v>2266</v>
       </c>
     </row>
     <row r="425" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -18995,7 +18998,7 @@
         <v>56</v>
       </c>
       <c r="H425" s="6" t="s">
-        <v>2268</v>
+        <v>2267</v>
       </c>
     </row>
     <row r="426" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -19074,7 +19077,7 @@
       </c>
       <c r="H428" s="17"/>
       <c r="J428" s="14" t="s">
-        <v>2266</v>
+        <v>2265</v>
       </c>
     </row>
     <row r="429" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -19100,7 +19103,7 @@
         <v>7</v>
       </c>
       <c r="H429" s="6" t="s">
-        <v>2269</v>
+        <v>2268</v>
       </c>
     </row>
     <row r="430" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -19126,7 +19129,7 @@
         <v>11</v>
       </c>
       <c r="H430" s="6" t="s">
-        <v>2270</v>
+        <v>2269</v>
       </c>
     </row>
     <row r="431" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -19202,7 +19205,7 @@
         <v>56</v>
       </c>
       <c r="H433" s="6" t="s">
-        <v>2271</v>
+        <v>2270</v>
       </c>
     </row>
     <row r="434" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -19621,7 +19624,7 @@
         <v>56</v>
       </c>
       <c r="J449" s="14" t="s">
-        <v>2266</v>
+        <v>2265</v>
       </c>
     </row>
     <row r="450" spans="1:10" ht="72" x14ac:dyDescent="0.3">
@@ -19646,9 +19649,11 @@
       <c r="G450" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="H450" s="17"/>
+      <c r="H450" s="22" t="s">
+        <v>2494</v>
+      </c>
       <c r="J450" s="11" t="s">
-        <v>2215</v>
+        <v>2214</v>
       </c>
     </row>
     <row r="451" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -19858,9 +19863,7 @@
       <c r="H458" s="6" t="s">
         <v>2194</v>
       </c>
-      <c r="I458" s="10" t="s">
-        <v>2195</v>
-      </c>
+      <c r="I458" s="10"/>
     </row>
     <row r="459" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A459" s="2" t="s">
@@ -19885,7 +19888,7 @@
         <v>56</v>
       </c>
       <c r="H459" s="6" t="s">
-        <v>2196</v>
+        <v>2195</v>
       </c>
     </row>
     <row r="460" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -19911,7 +19914,7 @@
         <v>11</v>
       </c>
       <c r="H460" s="6" t="s">
-        <v>2197</v>
+        <v>2196</v>
       </c>
     </row>
     <row r="461" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -19937,7 +19940,7 @@
         <v>7</v>
       </c>
       <c r="H461" s="6" t="s">
-        <v>2198</v>
+        <v>2197</v>
       </c>
     </row>
     <row r="462" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -19963,7 +19966,7 @@
         <v>11</v>
       </c>
       <c r="H462" s="6" t="s">
-        <v>2199</v>
+        <v>2198</v>
       </c>
     </row>
     <row r="463" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -19989,7 +19992,7 @@
         <v>11</v>
       </c>
       <c r="H463" s="6" t="s">
-        <v>2200</v>
+        <v>2199</v>
       </c>
     </row>
     <row r="464" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -20093,7 +20096,7 @@
         <v>11</v>
       </c>
       <c r="H467" s="6" t="s">
-        <v>2201</v>
+        <v>2200</v>
       </c>
       <c r="I467" s="11"/>
     </row>
@@ -20120,7 +20123,7 @@
         <v>56</v>
       </c>
       <c r="H468" s="6" t="s">
-        <v>2202</v>
+        <v>2201</v>
       </c>
     </row>
     <row r="469" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -20146,7 +20149,7 @@
         <v>56</v>
       </c>
       <c r="H469" s="6" t="s">
-        <v>2203</v>
+        <v>2202</v>
       </c>
     </row>
     <row r="470" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -20224,7 +20227,7 @@
         <v>7</v>
       </c>
       <c r="H472" s="6" t="s">
-        <v>2204</v>
+        <v>2203</v>
       </c>
     </row>
     <row r="473" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -20276,7 +20279,7 @@
         <v>11</v>
       </c>
       <c r="H474" s="6" t="s">
-        <v>2205</v>
+        <v>2204</v>
       </c>
     </row>
     <row r="475" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -20302,7 +20305,7 @@
         <v>7</v>
       </c>
       <c r="H475" s="6" t="s">
-        <v>2206</v>
+        <v>2205</v>
       </c>
     </row>
     <row r="476" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -20328,7 +20331,7 @@
         <v>56</v>
       </c>
       <c r="H476" s="8" t="s">
-        <v>2207</v>
+        <v>2206</v>
       </c>
     </row>
     <row r="477" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -20354,10 +20357,10 @@
         <v>56</v>
       </c>
       <c r="H477" s="8" t="s">
-        <v>2208</v>
-      </c>
-    </row>
-    <row r="478" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+        <v>2207</v>
+      </c>
+    </row>
+    <row r="478" spans="1:10" ht="52.2" x14ac:dyDescent="0.3">
       <c r="A478" s="2" t="s">
         <v>1274</v>
       </c>
@@ -20379,9 +20382,11 @@
       <c r="G478" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="H478" s="17"/>
+      <c r="H478" s="22" t="s">
+        <v>2495</v>
+      </c>
       <c r="J478" s="20" t="s">
-        <v>2211</v>
+        <v>2210</v>
       </c>
     </row>
     <row r="479" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -20407,7 +20412,7 @@
         <v>11</v>
       </c>
       <c r="H479" s="8" t="s">
-        <v>2209</v>
+        <v>2208</v>
       </c>
     </row>
     <row r="480" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -20433,7 +20438,7 @@
         <v>11</v>
       </c>
       <c r="H480" s="8" t="s">
-        <v>2210</v>
+        <v>2209</v>
       </c>
     </row>
     <row r="481" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -20459,7 +20464,7 @@
         <v>7</v>
       </c>
       <c r="H481" s="9" t="s">
-        <v>2212</v>
+        <v>2211</v>
       </c>
     </row>
     <row r="482" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -20485,7 +20490,7 @@
         <v>56</v>
       </c>
       <c r="H482" s="8" t="s">
-        <v>2213</v>
+        <v>2212</v>
       </c>
     </row>
     <row r="483" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -20511,7 +20516,7 @@
         <v>56</v>
       </c>
       <c r="H483" s="8" t="s">
-        <v>2214</v>
+        <v>2213</v>
       </c>
     </row>
     <row r="484" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -20694,7 +20699,7 @@
       </c>
       <c r="H490" s="6"/>
       <c r="J490" s="14" t="s">
-        <v>2266</v>
+        <v>2265</v>
       </c>
     </row>
     <row r="491" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -20720,7 +20725,7 @@
         <v>56</v>
       </c>
       <c r="H491" s="8" t="s">
-        <v>2232</v>
+        <v>2231</v>
       </c>
     </row>
     <row r="492" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -20746,7 +20751,7 @@
         <v>56</v>
       </c>
       <c r="H492" s="8" t="s">
-        <v>2233</v>
+        <v>2232</v>
       </c>
     </row>
     <row r="493" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -20772,7 +20777,7 @@
         <v>11</v>
       </c>
       <c r="H493" s="8" t="s">
-        <v>2234</v>
+        <v>2233</v>
       </c>
     </row>
     <row r="494" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -20798,7 +20803,7 @@
         <v>11</v>
       </c>
       <c r="H494" s="8" t="s">
-        <v>2235</v>
+        <v>2234</v>
       </c>
     </row>
     <row r="495" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -20824,7 +20829,7 @@
         <v>7</v>
       </c>
       <c r="H495" s="9" t="s">
-        <v>2236</v>
+        <v>2235</v>
       </c>
     </row>
     <row r="496" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -20850,7 +20855,7 @@
         <v>56</v>
       </c>
       <c r="H496" s="8" t="s">
-        <v>2237</v>
+        <v>2236</v>
       </c>
     </row>
     <row r="497" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -20876,7 +20881,7 @@
         <v>56</v>
       </c>
       <c r="H497" s="8" t="s">
-        <v>2238</v>
+        <v>2237</v>
       </c>
     </row>
     <row r="498" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -20928,7 +20933,7 @@
         <v>11</v>
       </c>
       <c r="H499" s="6" t="s">
-        <v>2272</v>
+        <v>2271</v>
       </c>
     </row>
     <row r="500" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -20954,7 +20959,7 @@
         <v>28</v>
       </c>
       <c r="H500" s="6" t="s">
-        <v>2273</v>
+        <v>2272</v>
       </c>
     </row>
     <row r="501" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -20980,7 +20985,7 @@
         <v>28</v>
       </c>
       <c r="H501" s="6" t="s">
-        <v>2273</v>
+        <v>2272</v>
       </c>
     </row>
     <row r="502" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -21006,7 +21011,7 @@
         <v>11</v>
       </c>
       <c r="H502" s="6" t="s">
-        <v>2275</v>
+        <v>2274</v>
       </c>
     </row>
     <row r="503" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -21032,7 +21037,7 @@
         <v>28</v>
       </c>
       <c r="H503" s="6" t="s">
-        <v>2274</v>
+        <v>2273</v>
       </c>
     </row>
     <row r="504" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -21058,7 +21063,7 @@
         <v>28</v>
       </c>
       <c r="H504" s="6" t="s">
-        <v>2274</v>
+        <v>2273</v>
       </c>
     </row>
     <row r="505" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -21084,7 +21089,7 @@
         <v>11</v>
       </c>
       <c r="H505" s="6" t="s">
-        <v>2276</v>
+        <v>2275</v>
       </c>
     </row>
     <row r="506" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -21110,7 +21115,7 @@
         <v>28</v>
       </c>
       <c r="H506" s="6" t="s">
-        <v>2277</v>
+        <v>2276</v>
       </c>
     </row>
     <row r="507" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -21136,7 +21141,7 @@
         <v>28</v>
       </c>
       <c r="H507" s="6" t="s">
-        <v>2277</v>
+        <v>2276</v>
       </c>
     </row>
     <row r="508" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -21162,7 +21167,7 @@
         <v>11</v>
       </c>
       <c r="H508" s="6" t="s">
-        <v>2278</v>
+        <v>2277</v>
       </c>
     </row>
     <row r="509" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -21188,7 +21193,7 @@
         <v>28</v>
       </c>
       <c r="H509" s="6" t="s">
-        <v>2279</v>
+        <v>2278</v>
       </c>
     </row>
     <row r="510" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -21214,7 +21219,7 @@
         <v>28</v>
       </c>
       <c r="H510" s="6" t="s">
-        <v>2279</v>
+        <v>2278</v>
       </c>
     </row>
     <row r="511" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -21396,7 +21401,7 @@
         <v>7</v>
       </c>
       <c r="H517" s="6" t="s">
-        <v>2250</v>
+        <v>2249</v>
       </c>
     </row>
     <row r="518" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -21422,7 +21427,7 @@
         <v>7</v>
       </c>
       <c r="H518" s="6" t="s">
-        <v>2251</v>
+        <v>2250</v>
       </c>
     </row>
     <row r="519" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -21474,7 +21479,7 @@
         <v>7</v>
       </c>
       <c r="H520" s="6" t="s">
-        <v>2252</v>
+        <v>2251</v>
       </c>
     </row>
     <row r="521" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -21500,7 +21505,7 @@
         <v>11</v>
       </c>
       <c r="H521" s="6" t="s">
-        <v>2253</v>
+        <v>2252</v>
       </c>
     </row>
     <row r="522" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -21526,7 +21531,7 @@
         <v>11</v>
       </c>
       <c r="H522" s="6" t="s">
-        <v>2254</v>
+        <v>2253</v>
       </c>
     </row>
     <row r="523" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -21604,7 +21609,7 @@
         <v>11</v>
       </c>
       <c r="H525" s="6" t="s">
-        <v>2255</v>
+        <v>2254</v>
       </c>
     </row>
     <row r="526" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -21631,10 +21636,10 @@
       </c>
       <c r="H526" s="17"/>
       <c r="I526" s="6" t="s">
-        <v>2247</v>
+        <v>2246</v>
       </c>
       <c r="J526" s="20" t="s">
-        <v>2256</v>
+        <v>2255</v>
       </c>
     </row>
     <row r="527" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
@@ -21661,7 +21666,7 @@
       </c>
       <c r="H527" s="17"/>
       <c r="J527" s="21" t="s">
-        <v>2257</v>
+        <v>2256</v>
       </c>
     </row>
     <row r="528" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
@@ -21688,7 +21693,7 @@
       </c>
       <c r="H528" s="17"/>
       <c r="J528" s="21" t="s">
-        <v>2258</v>
+        <v>2257</v>
       </c>
     </row>
     <row r="529" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
@@ -21714,7 +21719,7 @@
         <v>11</v>
       </c>
       <c r="H529" s="6" t="s">
-        <v>2280</v>
+        <v>2279</v>
       </c>
       <c r="I529" s="6"/>
     </row>
@@ -21741,7 +21746,7 @@
         <v>11</v>
       </c>
       <c r="H530" s="6" t="s">
-        <v>2281</v>
+        <v>2280</v>
       </c>
     </row>
     <row r="531" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
@@ -21767,7 +21772,7 @@
         <v>11</v>
       </c>
       <c r="H531" s="6" t="s">
-        <v>2286</v>
+        <v>2285</v>
       </c>
     </row>
     <row r="532" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
@@ -21817,7 +21822,7 @@
         <v>56</v>
       </c>
       <c r="H533" s="8" t="s">
-        <v>2309</v>
+        <v>2308</v>
       </c>
     </row>
     <row r="534" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
@@ -21843,7 +21848,7 @@
         <v>7</v>
       </c>
       <c r="H534" s="9" t="s">
-        <v>2311</v>
+        <v>2310</v>
       </c>
     </row>
     <row r="535" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
@@ -21869,7 +21874,7 @@
         <v>7</v>
       </c>
       <c r="H535" s="9" t="s">
-        <v>2318</v>
+        <v>2317</v>
       </c>
     </row>
     <row r="536" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
@@ -21895,7 +21900,7 @@
         <v>7</v>
       </c>
       <c r="H536" s="9" t="s">
-        <v>2310</v>
+        <v>2309</v>
       </c>
     </row>
     <row r="537" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
@@ -22293,7 +22298,7 @@
         <v>56</v>
       </c>
       <c r="H553" s="6" t="s">
-        <v>2302</v>
+        <v>2301</v>
       </c>
     </row>
     <row r="554" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -22319,7 +22324,7 @@
         <v>7</v>
       </c>
       <c r="H554" s="9" t="s">
-        <v>2317</v>
+        <v>2316</v>
       </c>
     </row>
     <row r="555" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -22345,7 +22350,7 @@
         <v>56</v>
       </c>
       <c r="H555" s="6" t="s">
-        <v>2304</v>
+        <v>2303</v>
       </c>
     </row>
     <row r="556" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -22371,7 +22376,7 @@
         <v>7</v>
       </c>
       <c r="H556" s="9" t="s">
-        <v>2312</v>
+        <v>2311</v>
       </c>
     </row>
     <row r="557" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -22397,7 +22402,7 @@
         <v>11</v>
       </c>
       <c r="H557" s="6" t="s">
-        <v>2305</v>
+        <v>2304</v>
       </c>
     </row>
     <row r="558" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -22423,7 +22428,7 @@
         <v>56</v>
       </c>
       <c r="H558" s="6" t="s">
-        <v>2303</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="559" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -22449,7 +22454,7 @@
         <v>7</v>
       </c>
       <c r="H559" s="9" t="s">
-        <v>2313</v>
+        <v>2312</v>
       </c>
     </row>
     <row r="560" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -22475,7 +22480,7 @@
         <v>7</v>
       </c>
       <c r="H560" s="9" t="s">
-        <v>2315</v>
+        <v>2314</v>
       </c>
     </row>
     <row r="561" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -22501,7 +22506,7 @@
         <v>7</v>
       </c>
       <c r="H561" s="9" t="s">
-        <v>2314</v>
+        <v>2313</v>
       </c>
     </row>
     <row r="562" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -22528,7 +22533,7 @@
       </c>
       <c r="H562" s="17"/>
       <c r="J562" s="14" t="s">
-        <v>2383</v>
+        <v>2382</v>
       </c>
     </row>
     <row r="563" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -22770,7 +22775,7 @@
         <v>7</v>
       </c>
       <c r="H572" s="9" t="s">
-        <v>2308</v>
+        <v>2307</v>
       </c>
     </row>
     <row r="573" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -22796,7 +22801,7 @@
         <v>7</v>
       </c>
       <c r="H573" s="9" t="s">
-        <v>2307</v>
+        <v>2306</v>
       </c>
     </row>
     <row r="574" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -22822,7 +22827,7 @@
         <v>7</v>
       </c>
       <c r="H574" s="9" t="s">
-        <v>2316</v>
+        <v>2315</v>
       </c>
     </row>
     <row r="575" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -22871,7 +22876,7 @@
         <v>11</v>
       </c>
       <c r="H576" s="6" t="s">
-        <v>2306</v>
+        <v>2305</v>
       </c>
     </row>
     <row r="577" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -22897,7 +22902,7 @@
         <v>56</v>
       </c>
       <c r="J577" s="14" t="s">
-        <v>2266</v>
+        <v>2265</v>
       </c>
     </row>
     <row r="578" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -22923,7 +22928,7 @@
         <v>56</v>
       </c>
       <c r="H578" s="6" t="s">
-        <v>2301</v>
+        <v>2300</v>
       </c>
     </row>
     <row r="579" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -22949,7 +22954,7 @@
         <v>56</v>
       </c>
       <c r="H579" s="8" t="s">
-        <v>2354</v>
+        <v>2353</v>
       </c>
     </row>
     <row r="580" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -22975,7 +22980,7 @@
         <v>56</v>
       </c>
       <c r="H580" s="8" t="s">
-        <v>2357</v>
+        <v>2356</v>
       </c>
     </row>
     <row r="581" spans="1:10" x14ac:dyDescent="0.3">
@@ -23003,7 +23008,7 @@
       <c r="H581" s="17"/>
       <c r="I581" s="8"/>
       <c r="J581" s="14" t="s">
-        <v>2256</v>
+        <v>2255</v>
       </c>
     </row>
     <row r="582" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -23029,7 +23034,7 @@
         <v>7</v>
       </c>
       <c r="H582" s="8" t="s">
-        <v>2360</v>
+        <v>2359</v>
       </c>
     </row>
     <row r="583" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -23055,7 +23060,7 @@
         <v>7</v>
       </c>
       <c r="H583" s="9" t="s">
-        <v>2350</v>
+        <v>2349</v>
       </c>
     </row>
     <row r="584" spans="1:10" x14ac:dyDescent="0.3">
@@ -23104,7 +23109,7 @@
         <v>11</v>
       </c>
       <c r="H585" s="8" t="s">
-        <v>2358</v>
+        <v>2357</v>
       </c>
     </row>
     <row r="586" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -23130,7 +23135,7 @@
         <v>11</v>
       </c>
       <c r="H586" s="8" t="s">
-        <v>2359</v>
+        <v>2358</v>
       </c>
     </row>
     <row r="587" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -23179,7 +23184,7 @@
         <v>56</v>
       </c>
       <c r="H588" s="8" t="s">
-        <v>2346</v>
+        <v>2345</v>
       </c>
     </row>
     <row r="589" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -23229,7 +23234,7 @@
       </c>
       <c r="H590" s="17"/>
       <c r="J590" s="14" t="s">
-        <v>2256</v>
+        <v>2255</v>
       </c>
     </row>
     <row r="591" spans="1:10" x14ac:dyDescent="0.3">
@@ -23255,7 +23260,7 @@
         <v>56</v>
       </c>
       <c r="J591" s="14" t="s">
-        <v>2266</v>
+        <v>2265</v>
       </c>
     </row>
     <row r="592" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -23281,7 +23286,7 @@
         <v>56</v>
       </c>
       <c r="H592" s="8" t="s">
-        <v>2361</v>
+        <v>2360</v>
       </c>
     </row>
     <row r="593" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -23379,7 +23384,7 @@
         <v>56</v>
       </c>
       <c r="H596" s="8" t="s">
-        <v>2356</v>
+        <v>2355</v>
       </c>
     </row>
     <row r="597" spans="1:10" x14ac:dyDescent="0.3">
@@ -23428,7 +23433,7 @@
         <v>7</v>
       </c>
       <c r="H598" s="6" t="s">
-        <v>2348</v>
+        <v>2347</v>
       </c>
     </row>
     <row r="599" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
@@ -23454,7 +23459,7 @@
         <v>328</v>
       </c>
       <c r="H599" s="6" t="s">
-        <v>2352</v>
+        <v>2351</v>
       </c>
     </row>
     <row r="600" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -23480,7 +23485,7 @@
         <v>7</v>
       </c>
       <c r="H600" s="6" t="s">
-        <v>2351</v>
+        <v>2350</v>
       </c>
     </row>
     <row r="601" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -23506,7 +23511,7 @@
         <v>7</v>
       </c>
       <c r="H601" s="6" t="s">
-        <v>2349</v>
+        <v>2348</v>
       </c>
     </row>
     <row r="602" spans="1:10" x14ac:dyDescent="0.3">
@@ -23532,7 +23537,7 @@
         <v>56</v>
       </c>
       <c r="J602" s="14" t="s">
-        <v>2266</v>
+        <v>2265</v>
       </c>
     </row>
     <row r="603" spans="1:10" x14ac:dyDescent="0.3">
@@ -23604,7 +23609,7 @@
         <v>7</v>
       </c>
       <c r="H605" s="8" t="s">
-        <v>2355</v>
+        <v>2354</v>
       </c>
     </row>
     <row r="606" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -23630,7 +23635,7 @@
         <v>56</v>
       </c>
       <c r="H606" s="8" t="s">
-        <v>2353</v>
+        <v>2352</v>
       </c>
     </row>
     <row r="607" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -23725,7 +23730,7 @@
         <v>56</v>
       </c>
       <c r="H610" s="6" t="s">
-        <v>2347</v>
+        <v>2346</v>
       </c>
     </row>
     <row r="611" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -23797,7 +23802,7 @@
         <v>263</v>
       </c>
       <c r="H613" s="6" t="s">
-        <v>2345</v>
+        <v>2344</v>
       </c>
     </row>
     <row r="614" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -23823,7 +23828,7 @@
         <v>7</v>
       </c>
       <c r="H614" s="6" t="s">
-        <v>2344</v>
+        <v>2343</v>
       </c>
     </row>
     <row r="615" spans="1:10" x14ac:dyDescent="0.3">
@@ -23850,7 +23855,7 @@
       </c>
       <c r="H615" s="17"/>
       <c r="J615" s="14" t="s">
-        <v>2256</v>
+        <v>2255</v>
       </c>
     </row>
     <row r="616" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -23876,7 +23881,7 @@
         <v>328</v>
       </c>
       <c r="H616" s="6" t="s">
-        <v>2385</v>
+        <v>2384</v>
       </c>
     </row>
     <row r="617" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -23903,7 +23908,7 @@
       </c>
       <c r="H617" s="18"/>
       <c r="J617" s="20" t="s">
-        <v>2386</v>
+        <v>2385</v>
       </c>
     </row>
     <row r="618" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -23929,7 +23934,7 @@
         <v>328</v>
       </c>
       <c r="H618" s="6" t="s">
-        <v>2388</v>
+        <v>2387</v>
       </c>
     </row>
     <row r="619" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -23955,7 +23960,7 @@
         <v>328</v>
       </c>
       <c r="H619" s="6" t="s">
-        <v>2387</v>
+        <v>2386</v>
       </c>
     </row>
     <row r="620" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -23981,7 +23986,7 @@
         <v>328</v>
       </c>
       <c r="H620" s="6" t="s">
-        <v>2389</v>
+        <v>2388</v>
       </c>
     </row>
     <row r="621" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -24007,7 +24012,7 @@
         <v>11</v>
       </c>
       <c r="H621" s="6" t="s">
-        <v>2404</v>
+        <v>2403</v>
       </c>
       <c r="I621" s="6"/>
     </row>
@@ -24034,7 +24039,7 @@
         <v>11</v>
       </c>
       <c r="H622" s="6" t="s">
-        <v>2319</v>
+        <v>2318</v>
       </c>
     </row>
     <row r="623" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -24060,7 +24065,7 @@
         <v>7</v>
       </c>
       <c r="H623" s="6" t="s">
-        <v>2322</v>
+        <v>2321</v>
       </c>
     </row>
     <row r="624" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -24086,7 +24091,7 @@
         <v>7</v>
       </c>
       <c r="H624" s="6" t="s">
-        <v>2390</v>
+        <v>2389</v>
       </c>
     </row>
     <row r="625" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -24112,7 +24117,7 @@
         <v>11</v>
       </c>
       <c r="H625" s="12" t="s">
-        <v>2331</v>
+        <v>2330</v>
       </c>
     </row>
     <row r="626" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -24231,10 +24236,10 @@
       </c>
       <c r="H630" s="17"/>
       <c r="I630" s="6" t="s">
-        <v>2321</v>
+        <v>2320</v>
       </c>
       <c r="J630" s="20" t="s">
-        <v>2256</v>
+        <v>2255</v>
       </c>
     </row>
     <row r="631" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -24284,10 +24289,10 @@
       </c>
       <c r="H632" s="17"/>
       <c r="I632" s="6" t="s">
+        <v>2390</v>
+      </c>
+      <c r="J632" s="14" t="s">
         <v>2391</v>
-      </c>
-      <c r="J632" s="14" t="s">
-        <v>2392</v>
       </c>
     </row>
     <row r="633" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -24314,10 +24319,10 @@
       </c>
       <c r="H633" s="17"/>
       <c r="I633" s="6" t="s">
+        <v>2390</v>
+      </c>
+      <c r="J633" s="14" t="s">
         <v>2391</v>
-      </c>
-      <c r="J633" s="14" t="s">
-        <v>2392</v>
       </c>
     </row>
     <row r="634" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -24343,7 +24348,7 @@
         <v>11</v>
       </c>
       <c r="H634" s="12" t="s">
-        <v>2323</v>
+        <v>2322</v>
       </c>
     </row>
     <row r="635" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -24369,7 +24374,7 @@
         <v>11</v>
       </c>
       <c r="H635" s="6" t="s">
-        <v>2327</v>
+        <v>2326</v>
       </c>
     </row>
     <row r="636" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -24395,7 +24400,7 @@
         <v>11</v>
       </c>
       <c r="H636" s="6" t="s">
-        <v>2393</v>
+        <v>2392</v>
       </c>
     </row>
     <row r="637" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -24421,7 +24426,7 @@
         <v>11</v>
       </c>
       <c r="H637" s="6" t="s">
-        <v>2330</v>
+        <v>2329</v>
       </c>
     </row>
     <row r="638" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -24447,7 +24452,7 @@
         <v>11</v>
       </c>
       <c r="H638" s="6" t="s">
-        <v>2329</v>
+        <v>2328</v>
       </c>
     </row>
     <row r="639" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -24473,7 +24478,7 @@
         <v>11</v>
       </c>
       <c r="H639" s="6" t="s">
-        <v>2396</v>
+        <v>2395</v>
       </c>
     </row>
     <row r="640" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -24499,7 +24504,7 @@
         <v>11</v>
       </c>
       <c r="H640" s="6" t="s">
-        <v>2340</v>
+        <v>2339</v>
       </c>
     </row>
     <row r="641" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -24548,7 +24553,7 @@
         <v>7</v>
       </c>
       <c r="H642" s="6" t="s">
-        <v>2397</v>
+        <v>2396</v>
       </c>
     </row>
     <row r="643" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -24574,7 +24579,7 @@
         <v>11</v>
       </c>
       <c r="H643" s="12" t="s">
-        <v>2325</v>
+        <v>2324</v>
       </c>
     </row>
     <row r="644" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -24600,7 +24605,7 @@
         <v>11</v>
       </c>
       <c r="H644" s="12" t="s">
-        <v>2324</v>
+        <v>2323</v>
       </c>
     </row>
     <row r="645" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -24810,7 +24815,7 @@
         <v>11</v>
       </c>
       <c r="H653" s="6" t="s">
-        <v>2398</v>
+        <v>2397</v>
       </c>
     </row>
     <row r="654" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -24836,7 +24841,7 @@
         <v>7</v>
       </c>
       <c r="H654" s="6" t="s">
-        <v>2400</v>
+        <v>2399</v>
       </c>
     </row>
     <row r="655" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -24862,7 +24867,7 @@
         <v>11</v>
       </c>
       <c r="H655" s="6" t="s">
-        <v>2337</v>
+        <v>2336</v>
       </c>
     </row>
     <row r="656" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -24912,7 +24917,7 @@
         <v>11</v>
       </c>
       <c r="H657" s="6" t="s">
-        <v>2401</v>
+        <v>2400</v>
       </c>
     </row>
     <row r="658" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -24938,7 +24943,7 @@
         <v>11</v>
       </c>
       <c r="H658" s="6" t="s">
-        <v>2403</v>
+        <v>2402</v>
       </c>
     </row>
     <row r="659" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -24964,7 +24969,7 @@
         <v>11</v>
       </c>
       <c r="H659" s="6" t="s">
-        <v>2399</v>
+        <v>2398</v>
       </c>
     </row>
     <row r="660" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -24990,7 +24995,7 @@
         <v>11</v>
       </c>
       <c r="H660" s="8" t="s">
-        <v>2405</v>
+        <v>2404</v>
       </c>
     </row>
     <row r="661" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -25063,7 +25068,7 @@
         <v>11</v>
       </c>
       <c r="H663" s="8" t="s">
-        <v>2406</v>
+        <v>2405</v>
       </c>
     </row>
     <row r="664" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -25089,7 +25094,7 @@
         <v>11</v>
       </c>
       <c r="H664" s="6" t="s">
-        <v>2407</v>
+        <v>2406</v>
       </c>
     </row>
     <row r="665" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -25115,7 +25120,7 @@
         <v>11</v>
       </c>
       <c r="H665" s="6" t="s">
-        <v>2326</v>
+        <v>2325</v>
       </c>
     </row>
     <row r="666" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -25141,7 +25146,7 @@
         <v>11</v>
       </c>
       <c r="H666" s="6" t="s">
-        <v>2394</v>
+        <v>2393</v>
       </c>
     </row>
     <row r="667" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -25167,7 +25172,7 @@
         <v>11</v>
       </c>
       <c r="H667" s="6" t="s">
-        <v>2283</v>
+        <v>2282</v>
       </c>
     </row>
     <row r="668" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -25193,7 +25198,7 @@
         <v>11</v>
       </c>
       <c r="H668" s="6" t="s">
-        <v>2282</v>
+        <v>2281</v>
       </c>
     </row>
     <row r="669" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -25220,10 +25225,10 @@
       </c>
       <c r="H669" s="17"/>
       <c r="I669" s="6" t="s">
-        <v>2321</v>
+        <v>2320</v>
       </c>
       <c r="J669" s="14" t="s">
-        <v>2256</v>
+        <v>2255</v>
       </c>
     </row>
     <row r="670" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -25249,7 +25254,7 @@
         <v>11</v>
       </c>
       <c r="H670" s="6" t="s">
-        <v>2339</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="671" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -25275,7 +25280,7 @@
         <v>28</v>
       </c>
       <c r="H671" s="9" t="s">
-        <v>2384</v>
+        <v>2383</v>
       </c>
     </row>
     <row r="672" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -25301,7 +25306,7 @@
         <v>56</v>
       </c>
       <c r="J672" s="14" t="s">
-        <v>2266</v>
+        <v>2265</v>
       </c>
     </row>
     <row r="673" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -25327,7 +25332,7 @@
         <v>56</v>
       </c>
       <c r="H673" s="12" t="s">
-        <v>2342</v>
+        <v>2341</v>
       </c>
     </row>
     <row r="674" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -25353,7 +25358,7 @@
         <v>11</v>
       </c>
       <c r="H674" s="6" t="s">
-        <v>2338</v>
+        <v>2337</v>
       </c>
     </row>
     <row r="675" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -25402,7 +25407,7 @@
         <v>11</v>
       </c>
       <c r="H676" s="6" t="s">
-        <v>2402</v>
+        <v>2401</v>
       </c>
     </row>
     <row r="677" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -25428,7 +25433,7 @@
         <v>7</v>
       </c>
       <c r="H677" s="6" t="s">
-        <v>2408</v>
+        <v>2407</v>
       </c>
     </row>
     <row r="678" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -25454,7 +25459,7 @@
         <v>7</v>
       </c>
       <c r="H678" s="6" t="s">
-        <v>2409</v>
+        <v>2408</v>
       </c>
     </row>
     <row r="679" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -25503,7 +25508,7 @@
         <v>56</v>
       </c>
       <c r="H680" s="6" t="s">
-        <v>2410</v>
+        <v>2409</v>
       </c>
     </row>
     <row r="681" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -25529,7 +25534,7 @@
         <v>11</v>
       </c>
       <c r="H681" s="6" t="s">
-        <v>2411</v>
+        <v>2410</v>
       </c>
     </row>
     <row r="682" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -25555,7 +25560,7 @@
         <v>7</v>
       </c>
       <c r="H682" s="6" t="s">
-        <v>2412</v>
+        <v>2411</v>
       </c>
     </row>
     <row r="683" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -25604,7 +25609,7 @@
         <v>56</v>
       </c>
       <c r="J684" s="14" t="s">
-        <v>2266</v>
+        <v>2265</v>
       </c>
     </row>
     <row r="685" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -25630,7 +25635,7 @@
         <v>56</v>
       </c>
       <c r="H685" s="6" t="s">
-        <v>2413</v>
+        <v>2412</v>
       </c>
     </row>
     <row r="686" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -25679,7 +25684,7 @@
         <v>28</v>
       </c>
       <c r="H687" s="9" t="s">
-        <v>2384</v>
+        <v>2383</v>
       </c>
     </row>
     <row r="688" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
@@ -25729,7 +25734,7 @@
       </c>
       <c r="H689" s="17"/>
       <c r="J689" s="14" t="s">
-        <v>2414</v>
+        <v>2413</v>
       </c>
     </row>
     <row r="690" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -25875,7 +25880,7 @@
         <v>11</v>
       </c>
       <c r="H695" s="12" t="s">
-        <v>2335</v>
+        <v>2334</v>
       </c>
     </row>
     <row r="696" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -25901,7 +25906,7 @@
         <v>7</v>
       </c>
       <c r="H696" s="6" t="s">
-        <v>2336</v>
+        <v>2335</v>
       </c>
     </row>
     <row r="697" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -25951,7 +25956,7 @@
         <v>7</v>
       </c>
       <c r="H698" s="6" t="s">
-        <v>2415</v>
+        <v>2414</v>
       </c>
     </row>
     <row r="699" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -25977,7 +25982,7 @@
         <v>7</v>
       </c>
       <c r="H699" s="6" t="s">
-        <v>2229</v>
+        <v>2228</v>
       </c>
     </row>
     <row r="700" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -26003,7 +26008,7 @@
         <v>7</v>
       </c>
       <c r="H700" s="12" t="s">
-        <v>2320</v>
+        <v>2319</v>
       </c>
     </row>
     <row r="701" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -26029,7 +26034,7 @@
         <v>7</v>
       </c>
       <c r="H701" s="6" t="s">
-        <v>2416</v>
+        <v>2415</v>
       </c>
     </row>
     <row r="702" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -26055,7 +26060,7 @@
         <v>11</v>
       </c>
       <c r="H702" s="12" t="s">
-        <v>2332</v>
+        <v>2331</v>
       </c>
     </row>
     <row r="703" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -26081,7 +26086,7 @@
         <v>11</v>
       </c>
       <c r="H703" s="12" t="s">
-        <v>2333</v>
+        <v>2332</v>
       </c>
     </row>
     <row r="704" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -26107,7 +26112,7 @@
         <v>11</v>
       </c>
       <c r="H704" s="12" t="s">
-        <v>2334</v>
+        <v>2333</v>
       </c>
     </row>
     <row r="705" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -26133,7 +26138,7 @@
         <v>328</v>
       </c>
       <c r="H705" s="12" t="s">
-        <v>2343</v>
+        <v>2342</v>
       </c>
     </row>
     <row r="706" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -26253,7 +26258,7 @@
         <v>11</v>
       </c>
       <c r="H710" s="6" t="s">
-        <v>2328</v>
+        <v>2327</v>
       </c>
     </row>
     <row r="711" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -26279,7 +26284,7 @@
         <v>11</v>
       </c>
       <c r="H711" s="6" t="s">
-        <v>2395</v>
+        <v>2394</v>
       </c>
     </row>
     <row r="712" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -26305,7 +26310,7 @@
         <v>11</v>
       </c>
       <c r="H712" s="6" t="s">
-        <v>2280</v>
+        <v>2279</v>
       </c>
     </row>
     <row r="713" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -26331,7 +26336,7 @@
         <v>11</v>
       </c>
       <c r="H713" s="6" t="s">
-        <v>2281</v>
+        <v>2280</v>
       </c>
     </row>
     <row r="714" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -26358,10 +26363,10 @@
       </c>
       <c r="H714" s="17"/>
       <c r="I714" s="6" t="s">
-        <v>2321</v>
+        <v>2320</v>
       </c>
       <c r="J714" s="14" t="s">
-        <v>2256</v>
+        <v>2255</v>
       </c>
     </row>
     <row r="715" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -26387,7 +26392,7 @@
         <v>11</v>
       </c>
       <c r="H715" s="6" t="s">
-        <v>2341</v>
+        <v>2340</v>
       </c>
     </row>
     <row r="716" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -26437,7 +26442,7 @@
         <v>28</v>
       </c>
       <c r="H717" s="6" t="s">
-        <v>2297</v>
+        <v>2296</v>
       </c>
     </row>
     <row r="718" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -26463,7 +26468,7 @@
         <v>56</v>
       </c>
       <c r="H718" s="6" t="s">
-        <v>2299</v>
+        <v>2298</v>
       </c>
     </row>
     <row r="719" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -26489,7 +26494,7 @@
         <v>28</v>
       </c>
       <c r="H719" s="6" t="s">
-        <v>2297</v>
+        <v>2296</v>
       </c>
     </row>
     <row r="720" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -26515,7 +26520,7 @@
         <v>28</v>
       </c>
       <c r="H720" s="6" t="s">
-        <v>2297</v>
+        <v>2296</v>
       </c>
     </row>
     <row r="721" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -26541,7 +26546,7 @@
         <v>28</v>
       </c>
       <c r="H721" s="6" t="s">
-        <v>2297</v>
+        <v>2296</v>
       </c>
     </row>
     <row r="722" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -26567,7 +26572,7 @@
         <v>28</v>
       </c>
       <c r="H722" s="6" t="s">
-        <v>2297</v>
+        <v>2296</v>
       </c>
     </row>
     <row r="723" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -26593,7 +26598,7 @@
         <v>28</v>
       </c>
       <c r="H723" s="6" t="s">
-        <v>2297</v>
+        <v>2296</v>
       </c>
     </row>
     <row r="724" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -26619,7 +26624,7 @@
         <v>28</v>
       </c>
       <c r="H724" s="6" t="s">
-        <v>2297</v>
+        <v>2296</v>
       </c>
     </row>
     <row r="725" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -26645,7 +26650,7 @@
         <v>28</v>
       </c>
       <c r="H725" s="6" t="s">
-        <v>2297</v>
+        <v>2296</v>
       </c>
     </row>
     <row r="726" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -26671,7 +26676,7 @@
         <v>56</v>
       </c>
       <c r="H726" s="6" t="s">
-        <v>2300</v>
+        <v>2299</v>
       </c>
     </row>
     <row r="727" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -26697,7 +26702,7 @@
         <v>28</v>
       </c>
       <c r="H727" s="6" t="s">
-        <v>2298</v>
+        <v>2297</v>
       </c>
     </row>
     <row r="728" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -26723,7 +26728,7 @@
         <v>28</v>
       </c>
       <c r="H728" s="6" t="s">
-        <v>2298</v>
+        <v>2297</v>
       </c>
     </row>
     <row r="729" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -26749,7 +26754,7 @@
         <v>28</v>
       </c>
       <c r="H729" s="6" t="s">
-        <v>2298</v>
+        <v>2297</v>
       </c>
     </row>
     <row r="730" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -26775,7 +26780,7 @@
         <v>28</v>
       </c>
       <c r="H730" s="6" t="s">
-        <v>2298</v>
+        <v>2297</v>
       </c>
     </row>
     <row r="731" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -26801,7 +26806,7 @@
         <v>28</v>
       </c>
       <c r="H731" s="6" t="s">
-        <v>2298</v>
+        <v>2297</v>
       </c>
     </row>
     <row r="732" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -26827,7 +26832,7 @@
         <v>28</v>
       </c>
       <c r="H732" s="6" t="s">
-        <v>2298</v>
+        <v>2297</v>
       </c>
     </row>
     <row r="733" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -26853,7 +26858,7 @@
         <v>28</v>
       </c>
       <c r="H733" s="6" t="s">
-        <v>2298</v>
+        <v>2297</v>
       </c>
     </row>
     <row r="734" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -26879,7 +26884,7 @@
         <v>28</v>
       </c>
       <c r="H734" s="6" t="s">
-        <v>2298</v>
+        <v>2297</v>
       </c>
     </row>
     <row r="735" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -26905,7 +26910,7 @@
         <v>7</v>
       </c>
       <c r="H735" s="6" t="s">
-        <v>2365</v>
+        <v>2364</v>
       </c>
     </row>
     <row r="736" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -26931,7 +26936,7 @@
         <v>7</v>
       </c>
       <c r="H736" s="6" t="s">
-        <v>2366</v>
+        <v>2365</v>
       </c>
     </row>
     <row r="737" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -26957,7 +26962,7 @@
         <v>7</v>
       </c>
       <c r="H737" s="6" t="s">
-        <v>2368</v>
+        <v>2367</v>
       </c>
     </row>
     <row r="738" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -26983,7 +26988,7 @@
         <v>7</v>
       </c>
       <c r="H738" s="6" t="s">
-        <v>2369</v>
+        <v>2368</v>
       </c>
     </row>
     <row r="739" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -27009,7 +27014,7 @@
         <v>7</v>
       </c>
       <c r="H739" s="6" t="s">
-        <v>2370</v>
+        <v>2369</v>
       </c>
     </row>
     <row r="740" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -27035,7 +27040,7 @@
         <v>7</v>
       </c>
       <c r="H740" s="6" t="s">
-        <v>2367</v>
+        <v>2366</v>
       </c>
     </row>
     <row r="741" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -27061,7 +27066,7 @@
         <v>7</v>
       </c>
       <c r="H741" s="6" t="s">
-        <v>2371</v>
+        <v>2370</v>
       </c>
     </row>
     <row r="742" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -27087,7 +27092,7 @@
         <v>28</v>
       </c>
       <c r="H742" s="6" t="s">
-        <v>2372</v>
+        <v>2371</v>
       </c>
     </row>
     <row r="743" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -27113,7 +27118,7 @@
         <v>28</v>
       </c>
       <c r="H743" s="6" t="s">
-        <v>2372</v>
+        <v>2371</v>
       </c>
     </row>
     <row r="744" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -27139,7 +27144,7 @@
         <v>28</v>
       </c>
       <c r="H744" s="6" t="s">
-        <v>2372</v>
+        <v>2371</v>
       </c>
     </row>
     <row r="745" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -27165,7 +27170,7 @@
         <v>28</v>
       </c>
       <c r="H745" s="6" t="s">
-        <v>2372</v>
+        <v>2371</v>
       </c>
     </row>
     <row r="746" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -27191,7 +27196,7 @@
         <v>28</v>
       </c>
       <c r="H746" s="6" t="s">
-        <v>2372</v>
+        <v>2371</v>
       </c>
     </row>
     <row r="747" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -27217,7 +27222,7 @@
         <v>28</v>
       </c>
       <c r="H747" s="6" t="s">
-        <v>2372</v>
+        <v>2371</v>
       </c>
     </row>
     <row r="748" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -27243,7 +27248,7 @@
         <v>28</v>
       </c>
       <c r="H748" s="6" t="s">
-        <v>2372</v>
+        <v>2371</v>
       </c>
     </row>
     <row r="749" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -27293,7 +27298,7 @@
         <v>28</v>
       </c>
       <c r="H750" s="6" t="s">
-        <v>2372</v>
+        <v>2371</v>
       </c>
     </row>
     <row r="751" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
@@ -27319,7 +27324,7 @@
         <v>11</v>
       </c>
       <c r="J751" s="14" t="s">
-        <v>2373</v>
+        <v>2372</v>
       </c>
     </row>
     <row r="752" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -27345,7 +27350,7 @@
         <v>56</v>
       </c>
       <c r="J752" s="14" t="s">
-        <v>2266</v>
+        <v>2265</v>
       </c>
     </row>
     <row r="753" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
@@ -27371,7 +27376,7 @@
         <v>56</v>
       </c>
       <c r="H753" s="6" t="s">
-        <v>2374</v>
+        <v>2373</v>
       </c>
     </row>
     <row r="754" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -27397,7 +27402,7 @@
         <v>56</v>
       </c>
       <c r="H754" s="6" t="s">
-        <v>2364</v>
+        <v>2363</v>
       </c>
     </row>
     <row r="755" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
@@ -27423,7 +27428,7 @@
         <v>28</v>
       </c>
       <c r="H755" s="6" t="s">
-        <v>2375</v>
+        <v>2374</v>
       </c>
     </row>
     <row r="756" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -27449,7 +27454,7 @@
         <v>56</v>
       </c>
       <c r="H756" s="6" t="s">
-        <v>2376</v>
+        <v>2375</v>
       </c>
     </row>
     <row r="757" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
@@ -27475,7 +27480,7 @@
         <v>28</v>
       </c>
       <c r="H757" s="6" t="s">
-        <v>2375</v>
+        <v>2374</v>
       </c>
     </row>
     <row r="758" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -27501,7 +27506,7 @@
         <v>56</v>
       </c>
       <c r="J758" s="14" t="s">
-        <v>2266</v>
+        <v>2265</v>
       </c>
     </row>
     <row r="759" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -27527,7 +27532,7 @@
         <v>7</v>
       </c>
       <c r="H759" s="6" t="s">
-        <v>2377</v>
+        <v>2376</v>
       </c>
     </row>
     <row r="760" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -27553,7 +27558,7 @@
         <v>56</v>
       </c>
       <c r="H760" s="6" t="s">
-        <v>2378</v>
+        <v>2377</v>
       </c>
     </row>
     <row r="761" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -27579,7 +27584,7 @@
         <v>7</v>
       </c>
       <c r="H761" s="6" t="s">
-        <v>2362</v>
+        <v>2361</v>
       </c>
     </row>
     <row r="762" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -27605,7 +27610,7 @@
         <v>7</v>
       </c>
       <c r="H762" s="6" t="s">
-        <v>2379</v>
+        <v>2378</v>
       </c>
     </row>
     <row r="763" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -27655,7 +27660,7 @@
         <v>28</v>
       </c>
       <c r="H764" s="6" t="s">
-        <v>2375</v>
+        <v>2374</v>
       </c>
     </row>
     <row r="765" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -27681,7 +27686,7 @@
         <v>56</v>
       </c>
       <c r="H765" s="6" t="s">
-        <v>2380</v>
+        <v>2379</v>
       </c>
     </row>
     <row r="766" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
@@ -27707,7 +27712,7 @@
         <v>28</v>
       </c>
       <c r="H766" s="6" t="s">
-        <v>2375</v>
+        <v>2374</v>
       </c>
     </row>
     <row r="767" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
@@ -27733,7 +27738,7 @@
         <v>28</v>
       </c>
       <c r="H767" s="6" t="s">
-        <v>2375</v>
+        <v>2374</v>
       </c>
     </row>
     <row r="768" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
@@ -27759,7 +27764,7 @@
         <v>28</v>
       </c>
       <c r="H768" s="6" t="s">
-        <v>2375</v>
+        <v>2374</v>
       </c>
     </row>
     <row r="769" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
@@ -27785,7 +27790,7 @@
         <v>28</v>
       </c>
       <c r="H769" s="6" t="s">
-        <v>2375</v>
+        <v>2374</v>
       </c>
     </row>
     <row r="770" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
@@ -27811,7 +27816,7 @@
         <v>28</v>
       </c>
       <c r="H770" s="6" t="s">
-        <v>2375</v>
+        <v>2374</v>
       </c>
     </row>
     <row r="771" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
@@ -27837,7 +27842,7 @@
         <v>28</v>
       </c>
       <c r="H771" s="6" t="s">
-        <v>2375</v>
+        <v>2374</v>
       </c>
     </row>
     <row r="772" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
@@ -27863,7 +27868,7 @@
         <v>28</v>
       </c>
       <c r="H772" s="6" t="s">
-        <v>2375</v>
+        <v>2374</v>
       </c>
     </row>
     <row r="773" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
@@ -27889,7 +27894,7 @@
         <v>28</v>
       </c>
       <c r="H773" s="6" t="s">
-        <v>2375</v>
+        <v>2374</v>
       </c>
     </row>
     <row r="774" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -27915,10 +27920,10 @@
         <v>11</v>
       </c>
       <c r="H774" s="6" t="s">
+        <v>2380</v>
+      </c>
+      <c r="J774" s="20" t="s">
         <v>2381</v>
-      </c>
-      <c r="J774" s="20" t="s">
-        <v>2382</v>
       </c>
     </row>
     <row r="775" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -27968,7 +27973,7 @@
         <v>7</v>
       </c>
       <c r="H776" s="6" t="s">
-        <v>2363</v>
+        <v>2362</v>
       </c>
     </row>
   </sheetData>

</xml_diff>